<commit_message>
Update template following recent changes
</commit_message>
<xml_diff>
--- a/admin/electionstemplate.xlsx
+++ b/admin/electionstemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents/camcycle/electionsurvey/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC39A06-0DB5-D648-A292-389F2595ACAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB368BB-E907-FD4B-BF03-76B179041D9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="3440" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="14" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>loony</t>
   </si>
@@ -160,12 +160,6 @@
     <t>Description of election</t>
   </si>
   <si>
-    <t>Division type, e.g. ward/division/constituency</t>
-  </si>
-  <si>
-    <t>Division type - plural, e.g. wards/divisions/constituencies</t>
-  </si>
-  <si>
     <t>Survey opening date</t>
   </si>
   <si>
@@ -203,12 +197,6 @@
   </si>
   <si>
     <t>Chairperson</t>
-  </si>
-  <si>
-    <t>Ward name prefix (if any)</t>
-  </si>
-  <si>
-    <t>Ward name</t>
   </si>
   <si>
     <t>District council</t>
@@ -277,9 +265,6 @@
     <t>Which election (matches ID in sheet 1)</t>
   </si>
   <si>
-    <t>Which ward (matches ID in sheet 2)</t>
-  </si>
-  <si>
     <t>You should probably aim to have max 6 or 7 questions for a survey - more than that is too long</t>
   </si>
   <si>
@@ -295,9 +280,6 @@
     <t>The rows along the top from Row C onwards are the question number (as in sheet 4), and you include that cell if you want it in a particular suvey. E.g. in the above example, Arbury gets questions 305-308, plus 313 and 315</t>
   </si>
   <si>
-    <t>The ward column should match the ID in sheet 2</t>
-  </si>
-  <si>
     <t>The affiliation (i.e. Party) should match the ID in sheet 3</t>
   </si>
   <si>
@@ -308,6 +290,36 @@
   </si>
   <si>
     <t>Reminder: make sure you check the existing database in the admin area webpage, as areas may already be defined from loading previous elections - you may not need to do this page, other than checking that all are present.</t>
+  </si>
+  <si>
+    <t>Type of electoral area, e.g. ward / division / constituency / Combined Authority area / area</t>
+  </si>
+  <si>
+    <t>Type of electoral area - plural, e.g. wards / divisions / constituencies / Combined Authority areas / areas</t>
+  </si>
+  <si>
+    <t>Area name</t>
+  </si>
+  <si>
+    <t>Area name prefix (if any)</t>
+  </si>
+  <si>
+    <t>Unique Area ID (areaId)</t>
+  </si>
+  <si>
+    <t>Which ward (matches Area ID in sheet 2)</t>
+  </si>
+  <si>
+    <t>areaId</t>
+  </si>
+  <si>
+    <t>The areaId column should match the Area ID values in sheet 2</t>
+  </si>
+  <si>
+    <t>If you don't know the address, just put a dash in the box: -</t>
+  </si>
+  <si>
+    <t>If you do know the address, it should be a single line with commas to separate each part of the address</t>
   </si>
 </sst>
 </file>
@@ -913,9 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBBCB1D-7DA7-904C-BDC3-26ABBF615D8F}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1047,12 +1057,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1075,7 @@
   <dimension ref="A1:M281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,34 +1107,34 @@
         <v>42</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="G1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1135,13 +1145,13 @@
         <v>14</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2" s="29">
         <v>42112</v>
@@ -1156,16 +1166,16 @@
         <v>42131</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
@@ -1237,12 +1247,12 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -1254,28 +1264,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1283,13 +1293,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -1302,12 +1312,12 @@
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1330,13 +1340,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1352,17 +1362,17 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1389,16 +1399,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1412,7 +1422,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1422,7 +1432,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1436,13 +1446,13 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.140625" style="6"/>
     <col min="6" max="6" width="12.7109375" style="6" customWidth="1"/>
     <col min="7" max="8" width="11.140625" style="6"/>
@@ -1453,10 +1463,10 @@
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1">
         <v>305</v>
@@ -1549,7 +1559,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1578,7 +1588,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -1604,19 +1614,19 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1627,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:XFB14"/>
+  <dimension ref="A1:XFB16"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,7 +1648,7 @@
     <col min="1" max="1" width="45.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="21" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" style="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="25" bestFit="1" customWidth="1"/>
@@ -1648,7 +1658,7 @@
   <sheetData>
     <row r="1" spans="1:16382" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>4</v>
@@ -1657,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>7</v>
@@ -1687,10 +1697,10 @@
         <v>11</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="6"/>
@@ -18070,17 +18080,27 @@
     </row>
     <row r="12" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16382" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16382" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>